<commit_message>
send unique data to each email
</commit_message>
<xml_diff>
--- a/front-end/src/assets/data/reservation00001.xlsx
+++ b/front-end/src/assets/data/reservation00001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\education\web_2023\hotel-reservation\front-end\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9B4024D-3E6B-454A-909F-9EEDB1B162F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927262C9-A30B-4E74-BD49-BE81E9482545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>d.chubenko996@gmail.com</t>
+  </si>
+  <si>
+    <t>zhekaprosto7@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -469,7 +472,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -565,7 +568,7 @@
         <v>210</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -679,7 +682,7 @@
         <v>205</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
@@ -717,7 +720,7 @@
         <v>203</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7" t="s">
         <v>8</v>
@@ -754,10 +757,10 @@
     <hyperlink ref="G2" r:id="rId6" xr:uid="{ED6B32EF-552D-466E-9F6D-C05CFAEA4243}"/>
     <hyperlink ref="D3" r:id="rId7" xr:uid="{EDFDFD92-9D46-4C35-B7AC-F4A10D1C0FEC}"/>
     <hyperlink ref="D4" r:id="rId8" xr:uid="{9D8BAA8C-ACCD-4DFE-9B3C-AB7A31FDC112}"/>
-    <hyperlink ref="D6" r:id="rId9" xr:uid="{0EC41114-575E-49E4-AC6D-7F359C21792F}"/>
-    <hyperlink ref="D7" r:id="rId10" xr:uid="{2A5BFAE9-2B63-439E-86B0-86ACC7C11F47}"/>
-    <hyperlink ref="D5" r:id="rId11" xr:uid="{30D24B89-541D-48ED-A07F-CBC4D7869DF3}"/>
-    <hyperlink ref="D2" r:id="rId12" xr:uid="{08A5EB92-620A-4973-A2D9-BB9E47BE445D}"/>
+    <hyperlink ref="D2" r:id="rId9" xr:uid="{08A5EB92-620A-4973-A2D9-BB9E47BE445D}"/>
+    <hyperlink ref="D5" r:id="rId10" xr:uid="{093DB701-8828-4EBB-B99E-6A17FBEBC07C}"/>
+    <hyperlink ref="D7" r:id="rId11" xr:uid="{FED30ADD-9CF0-48BC-8F22-16CD4E76D249}"/>
+    <hyperlink ref="D6" r:id="rId12" xr:uid="{F5FC2E76-3F60-4A1E-AFEE-EEF763A06CE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>